<commit_message>
Model accuracy page modified
</commit_message>
<xml_diff>
--- a/data/pivot.xlsx
+++ b/data/pivot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb95ccfb54cb50a2/Desktop/internship-project/project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_D0E6AF4B49C78FD20A103ECA7A66E7139C644225" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_D0E6AF4B49C78FD20A103ECA7A66E7139C644225" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{915597D9-8A2C-4D27-A5D9-7FC854F88F4C}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2892" yWindow="2772" windowWidth="17280" windowHeight="9420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Date Wise" sheetId="1" r:id="rId1"/>
@@ -1214,7 +1214,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A23" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -2627,11 +2627,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">

</xml_diff>